<commit_message>
vault backup: 2022-12-17 10:59:43
Affected files:
.obsidian/workspace.json
Университет/Учебные программы/ПИРСБД/Часы по дисциплинам.xlsx
</commit_message>
<xml_diff>
--- a/Университет/Учебные программы/ПИРСБД/Часы по дисциплинам.xlsx
+++ b/Университет/Учебные программы/ПИРСБД/Часы по дисциплинам.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cloud\knowledge-base\knowledge-base\Университет\Учебные программы\ПИРСБД\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B08CB366-8C2D-44B3-88A6-470D037F4914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DC9B86-BCBD-4547-8407-8F1B8562F21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E7A2B2EC-7D6E-4AFB-AAD1-DDD83F6F33AA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>Дисциплина</t>
   </si>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>Java для высоконагруженных вычислений</t>
+  </si>
+  <si>
+    <t>DevOPS</t>
+  </si>
+  <si>
+    <t>Форма контроля</t>
+  </si>
+  <si>
+    <t>Экз.</t>
+  </si>
+  <si>
+    <t>Зачет</t>
+  </si>
+  <si>
+    <t>Курсовая</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>Доп. Контроль</t>
+  </si>
+  <si>
+    <t>Проект</t>
+  </si>
+  <si>
+    <t>Факультативы</t>
   </si>
 </sst>
 </file>
@@ -480,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162E35EC-F593-445A-B8C2-3FAB66FAECA3}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,9 +520,11 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -511,8 +540,14 @@
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -521,7 +556,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -538,8 +573,14 @@
         <f>SUM(C3:D3)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -556,8 +597,14 @@
         <f t="shared" ref="E4:E6" si="0">SUM(C4:D4)</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -574,8 +621,14 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -592,8 +645,14 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7">
         <f>SUM(C3:C6)</f>
         <v>96</v>
@@ -607,7 +666,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -616,7 +675,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -633,8 +692,14 @@
         <f>SUM(C9:D9)</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -651,8 +716,14 @@
         <f t="shared" ref="E10:E13" si="1">SUM(C10:D10)</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -669,8 +740,14 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -681,14 +758,20 @@
         <v>16</v>
       </c>
       <c r="D12">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -699,28 +782,34 @@
         <v>16</v>
       </c>
       <c r="D13">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14">
         <f>SUM(C9:C13)</f>
         <v>112</v>
       </c>
       <c r="D14">
         <f>SUM(D9:D13)</f>
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="E14">
         <f>SUM(E9:E13)</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -729,7 +818,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -746,8 +835,14 @@
         <f t="shared" ref="E16:E23" si="2">SUM(C16:D16)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -764,8 +859,14 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -782,8 +883,14 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -800,8 +907,14 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -812,14 +925,20 @@
         <v>16</v>
       </c>
       <c r="D20">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -836,13 +955,19 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>16</v>
@@ -854,8 +979,14 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -866,32 +997,48 @@
         <v>16</v>
       </c>
       <c r="D23">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C24">
         <f>SUM(C16:C23)</f>
         <v>128</v>
       </c>
       <c r="D24">
         <f>SUM(D16:D23)</f>
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="E24">
         <f>SUM(E16:E23)</f>
-        <v>288</v>
-      </c>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A25:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>